<commit_message>
Overall reviewing of 'worklog.md' and attachments.
</commit_message>
<xml_diff>
--- a/app/Autorespond-config-OPS3.xlsx
+++ b/app/Autorespond-config-OPS3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Git\home\portable\repos\gmail-autoresponder-new\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Amine Data\Dev\gmail-autoresponder-new\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -60,13 +60,13 @@
     <t>(^|&lt;)(((mailer-daemon|postmaster)@.*)|((admin|boss|accounting|amine|noreply)@mycompany.*(.com|.biz|.info|.org|.net)))</t>
   </si>
   <si>
-    <t>(scammer|noreply|no-reply)|((^|&lt;)(ceo@spammer1.com|marketing@spammer2.com))</t>
-  </si>
-  <si>
     <t>(^|&lt;)((operations|operations2)@oldmailserver.com)</t>
   </si>
   <si>
     <t>(^|&lt;)((operations|operations2|noreply)@mycompany.*(.com|.biz|.info|.org|.net))</t>
+  </si>
+  <si>
+    <t>(scammer|noreply|no-reply|dot-not-reply)|((^|&lt;)(ceo@spammer1.com|marketing@spammer2.com))</t>
   </si>
 </sst>
 </file>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -419,10 +419,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
@@ -522,12 +522,12 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -557,7 +557,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>

</xml_diff>